<commit_message>
early exercise curve update
</commit_message>
<xml_diff>
--- a/Opgave 1.xlsx
+++ b/Opgave 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shark\source\repos\VNemirov\SaxoPUKCompFin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{525E78B0-0D72-4453-A0D9-3C7E6039AECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD705FA1-49F4-47B1-881D-FE8EADC43D55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="1185" windowWidth="36285" windowHeight="19665" firstSheet="1" activeTab="5" xr2:uid="{BC0D82F4-492A-4D65-855B-6D8E48A1622B}"/>
+    <workbookView xWindow="2115" yWindow="1320" windowWidth="36285" windowHeight="19665" firstSheet="1" activeTab="5" xr2:uid="{BC0D82F4-492A-4D65-855B-6D8E48A1622B}"/>
   </bookViews>
   <sheets>
     <sheet name="Calc_opg1_crank" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,6 @@
     <sheet name="Convergence" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029" calcOnSave="0"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +41,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -38000,10 +37999,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83D680DE-80A1-4AE5-B7E2-D89BB812F5C3}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38482,6 +38481,20 @@
         <v>-1.0915247251686122</v>
       </c>
     </row>
+    <row r="19" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <f>SLOPE(G2:G13,B2:B13)</f>
+        <v>-1.8842491298953825</v>
+      </c>
+      <c r="H19">
+        <f>SLOPE(H2:H13,B2:B13)</f>
+        <v>-1.0156003354891383</v>
+      </c>
+      <c r="I19">
+        <f>SLOPE(I6:I13,B6:B13)</f>
+        <v>-1.0571744279398998</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>